<commit_message>
fixed reading from and writing to Excel sheets with 16384 columns or 1048576 rows (Excel's maximum).
</commit_message>
<xml_diff>
--- a/larray/tests/test_blank_cells.xlsx
+++ b/larray/tests/test_blank_cells.xlsx
@@ -1,15 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="good" sheetId="77" r:id="rId1"/>
-    <sheet name="bad" sheetId="78" r:id="rId2"/>
-    <sheet name="bad2" sheetId="79" r:id="rId3"/>
+    <sheet name="blanksafter_morecolsthanrows" sheetId="78" r:id="rId2"/>
+    <sheet name="blanksafter_morerowsthancols" sheetId="83" r:id="rId3"/>
+    <sheet name="middleblankcol" sheetId="79" r:id="rId4"/>
+    <sheet name="16384col" sheetId="80" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="3">
   <si>
     <t>a\b</t>
   </si>
@@ -36,13 +38,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,12 +74,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,7 +445,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,10 +493,63 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A036406-58A0-4D7C-BE1D-C4959111924F}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="C1">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F597326E-5FAC-4D6B-9DF2-5793AF615EFD}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -539,4 +602,66 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2100F2CF-8F92-42E0-93CE-3661EFB506C2}">
+  <dimension ref="A1:XFD4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>2003</v>
+      </c>
+      <c r="C1">
+        <v>2004</v>
+      </c>
+      <c r="E1">
+        <v>2006</v>
+      </c>
+      <c r="XFD1" s="3"/>
+    </row>
+    <row r="2" spans="1:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="XFD2" s="3"/>
+    </row>
+    <row r="3" spans="1:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="XFD3" s="3"/>
+    </row>
+    <row r="4" spans="1:6 16384:16384" x14ac:dyDescent="0.25">
+      <c r="F4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>